<commit_message>
Updated BoM to reflect added capacitor.
</commit_message>
<xml_diff>
--- a/AssemblyBoM.xlsx
+++ b/AssemblyBoM.xlsx
@@ -190,10 +190,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -479,7 +479,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,17 +497,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -591,7 +591,7 @@
       <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>26</v>
       </c>
       <c r="H4" s="7">

</xml_diff>

<commit_message>
Cleaned up some unused cells in the BoM. Closes #1.
</commit_message>
<xml_diff>
--- a/AssemblyBoM.xlsx
+++ b/AssemblyBoM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Qty</t>
   </si>
@@ -63,12 +63,6 @@
   </si>
   <si>
     <t>Sensor Breakout Board V1.0</t>
-  </si>
-  <si>
-    <t>More economical to buy at least 50</t>
-  </si>
-  <si>
-    <t>Notes:</t>
   </si>
   <si>
     <t>MOLEX</t>
@@ -479,7 +473,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="K2" sqref="K2:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,37 +532,34 @@
         <v>8</v>
       </c>
       <c r="J2" s="8"/>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="3" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H3" s="7">
         <v>0.41</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J3" s="9"/>
     </row>
@@ -577,55 +568,53 @@
         <v>5</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H4" s="7">
         <v>0.46</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J4" s="9"/>
-      <c r="K4" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>32</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H5" s="7">
         <v>0.22</v>

</xml_diff>